<commit_message>
generated PA/YA weekly files, tested on week 1 data
</commit_message>
<xml_diff>
--- a/pointSettings.xlsx
+++ b/pointSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1083A263-9BD6-489D-8E54-5BBF088BDC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BAAB73-CC9C-4041-BF46-4A2CAC89D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
   <si>
     <t>Stat</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>D/ST</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>YA</t>
   </si>
 </sst>
 </file>
@@ -444,8 +450,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2D02E3B-FFDA-453D-A7A6-5C9EF84FFCB1}" name="ScoringTable" displayName="ScoringTable" ref="A1:D59" totalsRowShown="0">
-  <autoFilter ref="A1:D59" xr:uid="{F2D02E3B-FFDA-453D-A7A6-5C9EF84FFCB1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2D02E3B-FFDA-453D-A7A6-5C9EF84FFCB1}" name="ScoringTable" displayName="ScoringTable" ref="A1:D61" totalsRowShown="0">
+  <autoFilter ref="A1:D61" xr:uid="{F2D02E3B-FFDA-453D-A7A6-5C9EF84FFCB1}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{33FBEB08-3D36-4146-861D-D2CAE9A8DBF4}" name="Category"/>
     <tableColumn id="2" xr3:uid="{A631D2C3-3BA7-4ECA-A634-D172713EA25C}" name="Stat"/>
@@ -741,15 +747,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -763,7 +769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -777,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -791,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -805,7 +811,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -819,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -833,7 +839,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -847,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -861,7 +867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -875,7 +881,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -889,7 +895,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -903,7 +909,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -917,7 +923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -931,7 +937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -945,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -959,7 +965,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -973,7 +979,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -987,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>122</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>122</v>
       </c>
@@ -1211,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>122</v>
       </c>
@@ -1225,7 +1231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>122</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>122</v>
       </c>
@@ -1253,7 +1259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>122</v>
       </c>
@@ -1267,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>122</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>122</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -1365,7 +1371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>122</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -1407,7 +1413,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>122</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>122</v>
       </c>
@@ -1449,7 +1455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -1463,7 +1469,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -1477,7 +1483,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -1491,7 +1497,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>122</v>
       </c>
@@ -1505,7 +1511,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>122</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>122</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>122</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -1561,7 +1567,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -1575,10 +1581,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" t="s">
+        <v>124</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>